<commit_message>
Design moved to KiCad 6, counter logic fixed, extra display connector removed
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -544,12 +544,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -568,7 +580,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -578,6 +590,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -879,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -927,7 +942,7 @@
       <c r="C2" t="s">
         <v>88</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -947,7 +962,7 @@
       <c r="C3" t="s">
         <v>89</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -967,7 +982,7 @@
       <c r="C4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -987,7 +1002,7 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
@@ -1004,7 +1019,7 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1024,7 +1039,7 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1044,7 +1059,7 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1064,7 +1079,7 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1084,7 +1099,7 @@
       <c r="C10" t="s">
         <v>156</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1104,7 +1119,7 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1124,7 +1139,7 @@
       <c r="C12" t="s">
         <v>23</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1144,7 +1159,7 @@
       <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1164,7 +1179,7 @@
       <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="8" t="s">
         <v>142</v>
       </c>
       <c r="E14" s="1"/>
@@ -1219,7 +1234,7 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F17" t="s">
@@ -1239,7 +1254,7 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>154</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1259,7 +1274,7 @@
       <c r="C19" t="s">
         <v>93</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1279,7 +1294,7 @@
       <c r="C20" t="s">
         <v>94</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>143</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -1299,7 +1314,7 @@
       <c r="C21" t="s">
         <v>37</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F21" t="s">
@@ -1319,7 +1334,7 @@
       <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1339,7 +1354,7 @@
       <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>136</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -1359,7 +1374,7 @@
       <c r="C24" t="s">
         <v>130</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1379,7 +1394,7 @@
       <c r="C25" t="s">
         <v>134</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="7" t="s">
         <v>43</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1399,7 +1414,7 @@
       <c r="C26" t="s">
         <v>144</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="7" t="s">
         <v>44</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -1419,7 +1434,7 @@
       <c r="C27" t="s">
         <v>45</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1439,7 +1454,7 @@
       <c r="C28" t="s">
         <v>47</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="9" t="s">
         <v>48</v>
       </c>
       <c r="G28" t="s">
@@ -1456,7 +1471,7 @@
       <c r="C29" t="s">
         <v>95</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="7">
         <v>1.69</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -1476,7 +1491,7 @@
       <c r="C30" t="s">
         <v>49</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>50</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1496,7 +1511,7 @@
       <c r="C31" t="s">
         <v>138</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="7" t="s">
         <v>51</v>
       </c>
       <c r="F31" s="4" t="s">
@@ -1516,7 +1531,7 @@
       <c r="C32" t="s">
         <v>96</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="7" t="s">
         <v>52</v>
       </c>
       <c r="F32" s="2" t="s">
@@ -1536,7 +1551,7 @@
       <c r="C33" t="s">
         <v>53</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="7" t="s">
         <v>54</v>
       </c>
       <c r="F33" s="2" t="s">
@@ -1556,7 +1571,7 @@
       <c r="C34" t="s">
         <v>55</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E34">
@@ -1579,7 +1594,7 @@
       <c r="C35" t="s">
         <v>58</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="7" t="s">
         <v>59</v>
       </c>
       <c r="E35">
@@ -1602,7 +1617,7 @@
       <c r="C36" t="s">
         <v>61</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E36">
@@ -1625,7 +1640,7 @@
       <c r="C37" t="s">
         <v>97</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E37">
@@ -1671,7 +1686,7 @@
       <c r="C39" t="s">
         <v>69</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E39">
@@ -1694,7 +1709,7 @@
       <c r="C40" t="s">
         <v>72</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E40">
@@ -1717,7 +1732,7 @@
       <c r="C41" t="s">
         <v>98</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="7">
         <v>4028</v>
       </c>
       <c r="E41">
@@ -1740,7 +1755,7 @@
       <c r="C42" t="s">
         <v>99</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="7" t="s">
         <v>76</v>
       </c>
       <c r="E42">
@@ -1783,7 +1798,7 @@
       <c r="C44" t="s">
         <v>80</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="7" t="s">
         <v>81</v>
       </c>
       <c r="F44" s="2" t="s">
@@ -1803,7 +1818,7 @@
       <c r="C45" t="s">
         <v>83</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="7" t="s">
         <v>84</v>
       </c>
       <c r="F45" s="2" t="s">
@@ -1823,7 +1838,7 @@
       <c r="C46" t="s">
         <v>86</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="7" t="s">
         <v>87</v>
       </c>
       <c r="F46" s="4" t="s">

</xml_diff>